<commit_message>
Add Cherry Orchid Farm Centered data
</commit_message>
<xml_diff>
--- a/datasets/satelliteData/satRgbFinal4.xlsx
+++ b/datasets/satelliteData/satRgbFinal4.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="156">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t xml:space="preserve">sat_label</t>
   </si>
@@ -147,6 +147,24 @@
     <t xml:space="preserve">gray57</t>
   </si>
   <si>
+    <t xml:space="preserve">farmCherryCentered</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/Imageomics/Andromeda/raw/main/datasets/satelliteData/farmCherryCentered.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Centered Cherry Orchid Farm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gray37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ivory4</t>
+  </si>
+  <si>
     <t xml:space="preserve">farmDblBrook</t>
   </si>
   <si>
@@ -162,9 +180,6 @@
     <t xml:space="preserve">gray12</t>
   </si>
   <si>
-    <t xml:space="preserve">ivory4</t>
-  </si>
-  <si>
     <t xml:space="preserve">farmLawrenceville</t>
   </si>
   <si>
@@ -346,9 +361,6 @@
   </si>
   <si>
     <t xml:space="preserve">gray38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">gray25</t>
   </si>
   <si>
     <t xml:space="preserve">univArtMuseum</t>
@@ -972,52 +984,52 @@
         <v>0.110102455024202</v>
       </c>
       <c r="Q2" t="n">
-        <v>0.204951708638044</v>
+        <v>0.205026088309992</v>
       </c>
       <c r="R2" t="n">
-        <v>0.361271490115523</v>
+        <v>0.361308599231987</v>
       </c>
       <c r="S2" t="n">
-        <v>0.103829285737177</v>
+        <v>0.103867775732119</v>
       </c>
       <c r="T2" t="n">
-        <v>0.602941124851978</v>
+        <v>0.602963350747492</v>
       </c>
       <c r="U2" t="n">
-        <v>0.312061512218915</v>
+        <v>0.312146773939751</v>
       </c>
       <c r="V2" t="n">
-        <v>0.454567598926795</v>
+        <v>0.454591348511041</v>
       </c>
       <c r="W2" t="n">
-        <v>0.176471605660498</v>
+        <v>0.176532864554553</v>
       </c>
       <c r="X2" t="n">
-        <v>0.584050677081246</v>
+        <v>0.584066426802438</v>
       </c>
       <c r="Y2" t="n">
-        <v>0.191569882362021</v>
+        <v>0.19160602306223</v>
       </c>
       <c r="Z2" t="n">
-        <v>0.272835318092153</v>
+        <v>0.272862389471827</v>
       </c>
       <c r="AA2" t="n">
-        <v>0.128496372697394</v>
+        <v>0.128522614738915</v>
       </c>
       <c r="AB2" t="n">
-        <v>0.515793847681763</v>
+        <v>0.51581498340931</v>
       </c>
       <c r="AC2" t="n">
-        <v>0.317409688390477</v>
+        <v>0.31728100009192</v>
       </c>
       <c r="AD2" t="n">
-        <v>0.315146612740142</v>
+        <v>0.315034470079971</v>
       </c>
       <c r="AE2" t="n">
-        <v>0.297610074455373</v>
+        <v>0.297863774243956</v>
       </c>
       <c r="AF2" t="n">
-        <v>0.0698336244140086</v>
+        <v>0.069820755584153</v>
       </c>
       <c r="AG2" t="s">
         <v>40</v>
@@ -1046,88 +1058,88 @@
         <v>39</v>
       </c>
       <c r="E3" t="n">
-        <v>40.354852</v>
+        <v>40.310457</v>
       </c>
       <c r="F3" t="n">
-        <v>-74.741672</v>
+        <v>-74.716234</v>
       </c>
       <c r="G3" t="n">
-        <v>40.365821</v>
+        <v>40.322663</v>
       </c>
       <c r="H3" t="n">
-        <v>-74.76289</v>
+        <v>-74.744577</v>
       </c>
       <c r="I3" t="n">
-        <v>40.345643</v>
+        <v>40.29975</v>
       </c>
       <c r="J3" t="n">
-        <v>-74.720636</v>
+        <v>-74.687793</v>
       </c>
       <c r="K3" t="n">
-        <v>0.2</v>
+        <v>0.231372549019608</v>
       </c>
       <c r="L3" t="n">
-        <v>0.140305689776759</v>
+        <v>0.140218399730106</v>
       </c>
       <c r="M3" t="n">
-        <v>0.301960784313725</v>
+        <v>0.325490196078431</v>
       </c>
       <c r="N3" t="n">
-        <v>0.133204833625633</v>
+        <v>0.13104148718146</v>
       </c>
       <c r="O3" t="n">
-        <v>0.180392156862745</v>
+        <v>0.231372549019608</v>
       </c>
       <c r="P3" t="n">
-        <v>0.111648483992764</v>
+        <v>0.101889365036802</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.199309015279848</v>
+        <v>0.218986199314068</v>
       </c>
       <c r="R3" t="n">
-        <v>0.0994302562110132</v>
+        <v>0.364305032703089</v>
       </c>
       <c r="S3" t="n">
-        <v>0.364574482063837</v>
+        <v>0.106401237594484</v>
       </c>
       <c r="T3" t="n">
-        <v>0.572685658040096</v>
+        <v>0.572907268130175</v>
       </c>
       <c r="U3" t="n">
-        <v>0.29651850645526</v>
+        <v>0.310514907921958</v>
       </c>
       <c r="V3" t="n">
-        <v>0.154561438070307</v>
+        <v>0.439734659684387</v>
       </c>
       <c r="W3" t="n">
-        <v>0.4389481099849</v>
+        <v>0.171405305928427</v>
       </c>
       <c r="X3" t="n">
-        <v>0.545817501010818</v>
+        <v>0.553887226662858</v>
       </c>
       <c r="Y3" t="n">
-        <v>0.179321881115105</v>
+        <v>0.22569825799227</v>
       </c>
       <c r="Z3" t="n">
-        <v>0.100856174315228</v>
+        <v>0.30064025181042</v>
       </c>
       <c r="AA3" t="n">
-        <v>0.279686866152169</v>
+        <v>0.153498179073282</v>
       </c>
       <c r="AB3" t="n">
-        <v>0.498396551419329</v>
+        <v>0.510657893539387</v>
       </c>
       <c r="AC3" t="n">
-        <v>0.390455005055612</v>
+        <v>0.336091552532402</v>
       </c>
       <c r="AD3" t="n">
-        <v>0.282154609798695</v>
+        <v>0.308521003768729</v>
       </c>
       <c r="AE3" t="n">
-        <v>0.264180531298833</v>
+        <v>0.288052210681129</v>
       </c>
       <c r="AF3" t="n">
-        <v>0.0632098538468609</v>
+        <v>0.0673352330177406</v>
       </c>
       <c r="AG3" t="s">
         <v>47</v>
@@ -1136,7 +1148,7 @@
         <v>48</v>
       </c>
       <c r="AI3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="AJ3" t="s">
         <v>49</v>
@@ -1156,100 +1168,100 @@
         <v>39</v>
       </c>
       <c r="E4" t="n">
-        <v>40.318704</v>
+        <v>40.354852</v>
       </c>
       <c r="F4" t="n">
-        <v>-74.744964</v>
+        <v>-74.741672</v>
       </c>
       <c r="G4" t="n">
-        <v>40.328533</v>
+        <v>40.365821</v>
       </c>
       <c r="H4" t="n">
-        <v>-74.765787</v>
+        <v>-74.76289</v>
       </c>
       <c r="I4" t="n">
-        <v>40.30969</v>
+        <v>40.345643</v>
       </c>
       <c r="J4" t="n">
-        <v>-74.723841</v>
+        <v>-74.720636</v>
       </c>
       <c r="K4" t="n">
-        <v>0.243137254901961</v>
+        <v>0.2</v>
       </c>
       <c r="L4" t="n">
-        <v>0.130786464345831</v>
+        <v>0.140305689776759</v>
       </c>
       <c r="M4" t="n">
-        <v>0.349019607843137</v>
+        <v>0.301960784313725</v>
       </c>
       <c r="N4" t="n">
-        <v>0.127349196548707</v>
+        <v>0.133204833625633</v>
       </c>
       <c r="O4" t="n">
-        <v>0.203921568627451</v>
+        <v>0.180392156862745</v>
       </c>
       <c r="P4" t="n">
-        <v>0.0926279896415932</v>
+        <v>0.111648483992764</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.341761781187704</v>
+        <v>0.199309015279848</v>
       </c>
       <c r="R4" t="n">
-        <v>0.193506370174901</v>
+        <v>0.0994302562110132</v>
       </c>
       <c r="S4" t="n">
-        <v>0.0985673297631171</v>
+        <v>0.364574482063837</v>
       </c>
       <c r="T4" t="n">
-        <v>0.551805091994163</v>
+        <v>0.572685658040096</v>
       </c>
       <c r="U4" t="n">
-        <v>0.441594237333882</v>
+        <v>0.29651850645526</v>
       </c>
       <c r="V4" t="n">
-        <v>0.301944337935679</v>
+        <v>0.154561438070307</v>
       </c>
       <c r="W4" t="n">
-        <v>0.171100168762641</v>
+        <v>0.4389481099849</v>
       </c>
       <c r="X4" t="n">
-        <v>0.542373134232376</v>
+        <v>0.545817501010818</v>
       </c>
       <c r="Y4" t="n">
-        <v>0.258447097760468</v>
+        <v>0.179321881115105</v>
       </c>
       <c r="Z4" t="n">
-        <v>0.184214404599468</v>
+        <v>0.100856174315228</v>
       </c>
       <c r="AA4" t="n">
-        <v>0.122766917951963</v>
+        <v>0.279686866152169</v>
       </c>
       <c r="AB4" t="n">
-        <v>0.476703387160047</v>
+        <v>0.498396551419329</v>
       </c>
       <c r="AC4" t="n">
-        <v>0.407344425039066</v>
+        <v>0.390455005055612</v>
       </c>
       <c r="AD4" t="n">
-        <v>0.30290651714312</v>
+        <v>0.282154609798695</v>
       </c>
       <c r="AE4" t="n">
-        <v>0.233696111774979</v>
+        <v>0.264180531298833</v>
       </c>
       <c r="AF4" t="n">
-        <v>0.0560529460428348</v>
+        <v>0.0632098538468609</v>
       </c>
       <c r="AG4" t="s">
+        <v>53</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI4" t="s">
         <v>41</v>
       </c>
-      <c r="AH4" t="s">
-        <v>47</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>53</v>
-      </c>
       <c r="AJ4" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="5">
@@ -1266,97 +1278,97 @@
         <v>39</v>
       </c>
       <c r="E5" t="n">
-        <v>40.352764</v>
+        <v>40.318704</v>
       </c>
       <c r="F5" t="n">
-        <v>-74.719865</v>
+        <v>-74.744964</v>
       </c>
       <c r="G5" t="n">
-        <v>40.363028</v>
+        <v>40.328533</v>
       </c>
       <c r="H5" t="n">
-        <v>-74.74057</v>
+        <v>-74.765787</v>
       </c>
       <c r="I5" t="n">
-        <v>40.342669</v>
+        <v>40.30969</v>
       </c>
       <c r="J5" t="n">
-        <v>-74.698661</v>
+        <v>-74.723841</v>
       </c>
       <c r="K5" t="n">
-        <v>0.188235294117647</v>
+        <v>0.243137254901961</v>
       </c>
       <c r="L5" t="n">
-        <v>0.138351991216952</v>
+        <v>0.130786464345831</v>
       </c>
       <c r="M5" t="n">
-        <v>0.282352941176471</v>
+        <v>0.349019607843137</v>
       </c>
       <c r="N5" t="n">
-        <v>0.134061992106156</v>
+        <v>0.127349196548707</v>
       </c>
       <c r="O5" t="n">
-        <v>0.172549019607843</v>
+        <v>0.203921568627451</v>
       </c>
       <c r="P5" t="n">
-        <v>0.108559691145135</v>
+        <v>0.0926279896415932</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.199146374695632</v>
+        <v>0.341761781187704</v>
       </c>
       <c r="R5" t="n">
-        <v>0.0986747809492752</v>
+        <v>0.193506370174901</v>
       </c>
       <c r="S5" t="n">
-        <v>0.370998162528187</v>
+        <v>0.0985673297631171</v>
       </c>
       <c r="T5" t="n">
-        <v>0.589293581623865</v>
+        <v>0.551805091994163</v>
       </c>
       <c r="U5" t="n">
-        <v>0.293962030251813</v>
+        <v>0.441594237333882</v>
       </c>
       <c r="V5" t="n">
-        <v>0.154170968148882</v>
+        <v>0.301944337935679</v>
       </c>
       <c r="W5" t="n">
-        <v>0.444230737084637</v>
+        <v>0.171100168762641</v>
       </c>
       <c r="X5" t="n">
-        <v>0.564326079821592</v>
+        <v>0.542373134232376</v>
       </c>
       <c r="Y5" t="n">
-        <v>0.180585158981223</v>
+        <v>0.258447097760468</v>
       </c>
       <c r="Z5" t="n">
-        <v>0.108536048177919</v>
+        <v>0.184214404599468</v>
       </c>
       <c r="AA5" t="n">
-        <v>0.278994443865823</v>
+        <v>0.122766917951963</v>
       </c>
       <c r="AB5" t="n">
-        <v>0.528382141541654</v>
+        <v>0.476703387160047</v>
       </c>
       <c r="AC5" t="n">
-        <v>0.402266752458866</v>
+        <v>0.407344425039066</v>
       </c>
       <c r="AD5" t="n">
-        <v>0.323160216931703</v>
+        <v>0.30290651714312</v>
       </c>
       <c r="AE5" t="n">
-        <v>0.224270613107822</v>
+        <v>0.233696111774979</v>
       </c>
       <c r="AF5" t="n">
-        <v>0.0503024175016086</v>
+        <v>0.0560529460428348</v>
       </c>
       <c r="AG5" t="s">
+        <v>41</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>53</v>
+      </c>
+      <c r="AI5" t="s">
         <v>58</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>48</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>41</v>
       </c>
       <c r="AJ5" t="s">
         <v>59</v>
@@ -1373,757 +1385,757 @@
         <v>62</v>
       </c>
       <c r="D6" t="s">
+        <v>39</v>
+      </c>
+      <c r="E6" t="n">
+        <v>40.352764</v>
+      </c>
+      <c r="F6" t="n">
+        <v>-74.719865</v>
+      </c>
+      <c r="G6" t="n">
+        <v>40.363028</v>
+      </c>
+      <c r="H6" t="n">
+        <v>-74.74057</v>
+      </c>
+      <c r="I6" t="n">
+        <v>40.342669</v>
+      </c>
+      <c r="J6" t="n">
+        <v>-74.698661</v>
+      </c>
+      <c r="K6" t="n">
+        <v>0.188235294117647</v>
+      </c>
+      <c r="L6" t="n">
+        <v>0.138351991216952</v>
+      </c>
+      <c r="M6" t="n">
+        <v>0.282352941176471</v>
+      </c>
+      <c r="N6" t="n">
+        <v>0.134061992106156</v>
+      </c>
+      <c r="O6" t="n">
+        <v>0.172549019607843</v>
+      </c>
+      <c r="P6" t="n">
+        <v>0.108559691145135</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>0.199128594056795</v>
+      </c>
+      <c r="R6" t="n">
+        <v>0.0986578692483058</v>
+      </c>
+      <c r="S6" t="n">
+        <v>0.370994227390301</v>
+      </c>
+      <c r="T6" t="n">
+        <v>0.589291249884452</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.293939119479546</v>
+      </c>
+      <c r="V6" t="n">
+        <v>0.154146748615205</v>
+      </c>
+      <c r="W6" t="n">
+        <v>0.444227711741093</v>
+      </c>
+      <c r="X6" t="n">
+        <v>0.56432466053702</v>
+      </c>
+      <c r="Y6" t="n">
+        <v>0.180576185040869</v>
+      </c>
+      <c r="Z6" t="n">
+        <v>0.108521132104084</v>
+      </c>
+      <c r="AA6" t="n">
+        <v>0.278990021530769</v>
+      </c>
+      <c r="AB6" t="n">
+        <v>0.528376446511068</v>
+      </c>
+      <c r="AC6" t="n">
+        <v>0.402373379906241</v>
+      </c>
+      <c r="AD6" t="n">
+        <v>0.323044397463002</v>
+      </c>
+      <c r="AE6" t="n">
+        <v>0.224277966724883</v>
+      </c>
+      <c r="AF6" t="n">
+        <v>0.0503042559058737</v>
+      </c>
+      <c r="AG6" t="s">
         <v>63</v>
       </c>
-      <c r="E6" t="n">
-        <v>40.365934</v>
-      </c>
-      <c r="F6" t="n">
-        <v>-74.672103</v>
-      </c>
-      <c r="G6" t="n">
-        <v>40.375474</v>
-      </c>
-      <c r="H6" t="n">
-        <v>-74.693112</v>
-      </c>
-      <c r="I6" t="n">
-        <v>40.356519</v>
-      </c>
-      <c r="J6" t="n">
-        <v>-74.650875</v>
-      </c>
-      <c r="K6" t="n">
-        <v>0.23921568627451</v>
-      </c>
-      <c r="L6" t="n">
-        <v>0.151668211990847</v>
-      </c>
-      <c r="M6" t="n">
-        <v>0.337254901960784</v>
-      </c>
-      <c r="N6" t="n">
-        <v>0.134945000466655</v>
-      </c>
-      <c r="O6" t="n">
-        <v>0.262745098039216</v>
-      </c>
-      <c r="P6" t="n">
-        <v>0.128232047892485</v>
-      </c>
-      <c r="Q6" t="n">
-        <v>0.242548455408818</v>
-      </c>
-      <c r="R6" t="n">
-        <v>0.138634005168871</v>
-      </c>
-      <c r="S6" t="n">
-        <v>0.414692065874519</v>
-      </c>
-      <c r="T6" t="n">
-        <v>0.621088129090767</v>
-      </c>
-      <c r="U6" t="n">
-        <v>0.341373922721555</v>
-      </c>
-      <c r="V6" t="n">
-        <v>0.20854198416251</v>
-      </c>
-      <c r="W6" t="n">
-        <v>0.472853186066329</v>
-      </c>
-      <c r="X6" t="n">
-        <v>0.617311226636281</v>
-      </c>
-      <c r="Y6" t="n">
-        <v>0.265514088680185</v>
-      </c>
-      <c r="Z6" t="n">
-        <v>0.19663082727455</v>
-      </c>
-      <c r="AA6" t="n">
-        <v>0.38434696661171</v>
-      </c>
-      <c r="AB6" t="n">
-        <v>0.616342684968064</v>
-      </c>
-      <c r="AC6" t="n">
-        <v>0.41145693538009</v>
-      </c>
-      <c r="AD6" t="n">
-        <v>0.288522842172994</v>
-      </c>
-      <c r="AE6" t="n">
-        <v>0.212111407298465</v>
-      </c>
-      <c r="AF6" t="n">
-        <v>0.0879088151484511</v>
-      </c>
-      <c r="AG6" t="s">
+      <c r="AH6" t="s">
+        <v>54</v>
+      </c>
+      <c r="AI6" t="s">
+        <v>41</v>
+      </c>
+      <c r="AJ6" t="s">
         <v>64</v>
-      </c>
-      <c r="AH6" t="s">
-        <v>65</v>
-      </c>
-      <c r="AI6" t="s">
-        <v>66</v>
-      </c>
-      <c r="AJ6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
+        <v>65</v>
+      </c>
+      <c r="B7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C7" t="s">
+        <v>67</v>
+      </c>
+      <c r="D7" t="s">
         <v>68</v>
       </c>
-      <c r="B7" t="s">
+      <c r="E7" t="n">
+        <v>40.365934</v>
+      </c>
+      <c r="F7" t="n">
+        <v>-74.672103</v>
+      </c>
+      <c r="G7" t="n">
+        <v>40.375474</v>
+      </c>
+      <c r="H7" t="n">
+        <v>-74.693112</v>
+      </c>
+      <c r="I7" t="n">
+        <v>40.356519</v>
+      </c>
+      <c r="J7" t="n">
+        <v>-74.650875</v>
+      </c>
+      <c r="K7" t="n">
+        <v>0.23921568627451</v>
+      </c>
+      <c r="L7" t="n">
+        <v>0.151668211990847</v>
+      </c>
+      <c r="M7" t="n">
+        <v>0.337254901960784</v>
+      </c>
+      <c r="N7" t="n">
+        <v>0.134945000466655</v>
+      </c>
+      <c r="O7" t="n">
+        <v>0.262745098039216</v>
+      </c>
+      <c r="P7" t="n">
+        <v>0.128232047892485</v>
+      </c>
+      <c r="Q7" t="n">
+        <v>0.242548455408818</v>
+      </c>
+      <c r="R7" t="n">
+        <v>0.138634005168871</v>
+      </c>
+      <c r="S7" t="n">
+        <v>0.414692065874519</v>
+      </c>
+      <c r="T7" t="n">
+        <v>0.621088129090767</v>
+      </c>
+      <c r="U7" t="n">
+        <v>0.341373922721555</v>
+      </c>
+      <c r="V7" t="n">
+        <v>0.20854198416251</v>
+      </c>
+      <c r="W7" t="n">
+        <v>0.472853186066329</v>
+      </c>
+      <c r="X7" t="n">
+        <v>0.617311226636281</v>
+      </c>
+      <c r="Y7" t="n">
+        <v>0.265514088680185</v>
+      </c>
+      <c r="Z7" t="n">
+        <v>0.19663082727455</v>
+      </c>
+      <c r="AA7" t="n">
+        <v>0.38434696661171</v>
+      </c>
+      <c r="AB7" t="n">
+        <v>0.616342684968064</v>
+      </c>
+      <c r="AC7" t="n">
+        <v>0.41145693538009</v>
+      </c>
+      <c r="AD7" t="n">
+        <v>0.288522842172994</v>
+      </c>
+      <c r="AE7" t="n">
+        <v>0.212111407298465</v>
+      </c>
+      <c r="AF7" t="n">
+        <v>0.0879088151484511</v>
+      </c>
+      <c r="AG7" t="s">
         <v>69</v>
       </c>
-      <c r="C7" t="s">
+      <c r="AH7" t="s">
         <v>70</v>
       </c>
-      <c r="D7" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" t="n">
-        <v>40.347059</v>
-      </c>
-      <c r="F7" t="n">
-        <v>-74.656342</v>
-      </c>
-      <c r="G7" t="n">
-        <v>40.356602</v>
-      </c>
-      <c r="H7" t="n">
-        <v>-74.677287</v>
-      </c>
-      <c r="I7" t="n">
-        <v>40.337598</v>
-      </c>
-      <c r="J7" t="n">
-        <v>-74.635291</v>
-      </c>
-      <c r="K7" t="n">
-        <v>0.301960784313725</v>
-      </c>
-      <c r="L7" t="n">
-        <v>0.164197797303097</v>
-      </c>
-      <c r="M7" t="n">
-        <v>0.380392156862745</v>
-      </c>
-      <c r="N7" t="n">
-        <v>0.144011195646163</v>
-      </c>
-      <c r="O7" t="n">
-        <v>0.313725490196078</v>
-      </c>
-      <c r="P7" t="n">
-        <v>0.137970565862388</v>
-      </c>
-      <c r="Q7" t="n">
-        <v>0.282255022459412</v>
-      </c>
-      <c r="R7" t="n">
-        <v>0.164893413158706</v>
-      </c>
-      <c r="S7" t="n">
-        <v>0.445943770310959</v>
-      </c>
-      <c r="T7" t="n">
-        <v>0.633076763588844</v>
-      </c>
-      <c r="U7" t="n">
-        <v>0.366396011516635</v>
-      </c>
-      <c r="V7" t="n">
-        <v>0.223571888867378</v>
-      </c>
-      <c r="W7" t="n">
-        <v>0.484556113960742</v>
-      </c>
-      <c r="X7" t="n">
-        <v>0.624276673154581</v>
-      </c>
-      <c r="Y7" t="n">
-        <v>0.303739821935569</v>
-      </c>
-      <c r="Z7" t="n">
-        <v>0.2316264693977</v>
-      </c>
-      <c r="AA7" t="n">
-        <v>0.42968802908603</v>
-      </c>
-      <c r="AB7" t="n">
-        <v>0.62359959476019</v>
-      </c>
-      <c r="AC7" t="n">
-        <v>0.332056255170512</v>
-      </c>
-      <c r="AD7" t="n">
-        <v>0.28310138799522</v>
-      </c>
-      <c r="AE7" t="n">
-        <v>0.250274841437632</v>
-      </c>
-      <c r="AF7" t="n">
-        <v>0.134567515396636</v>
-      </c>
-      <c r="AG7" t="s">
+      <c r="AI7" t="s">
         <v>71</v>
       </c>
-      <c r="AH7" t="s">
+      <c r="AJ7" t="s">
         <v>72</v>
-      </c>
-      <c r="AI7" t="s">
-        <v>73</v>
-      </c>
-      <c r="AJ7" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
         <v>75</v>
       </c>
-      <c r="B8" t="s">
+      <c r="D8" t="s">
+        <v>68</v>
+      </c>
+      <c r="E8" t="n">
+        <v>40.347059</v>
+      </c>
+      <c r="F8" t="n">
+        <v>-74.656342</v>
+      </c>
+      <c r="G8" t="n">
+        <v>40.356602</v>
+      </c>
+      <c r="H8" t="n">
+        <v>-74.677287</v>
+      </c>
+      <c r="I8" t="n">
+        <v>40.337598</v>
+      </c>
+      <c r="J8" t="n">
+        <v>-74.635291</v>
+      </c>
+      <c r="K8" t="n">
+        <v>0.301960784313725</v>
+      </c>
+      <c r="L8" t="n">
+        <v>0.164197797303097</v>
+      </c>
+      <c r="M8" t="n">
+        <v>0.380392156862745</v>
+      </c>
+      <c r="N8" t="n">
+        <v>0.144011195646163</v>
+      </c>
+      <c r="O8" t="n">
+        <v>0.313725490196078</v>
+      </c>
+      <c r="P8" t="n">
+        <v>0.137970565862388</v>
+      </c>
+      <c r="Q8" t="n">
+        <v>0.282255022459412</v>
+      </c>
+      <c r="R8" t="n">
+        <v>0.164893413158706</v>
+      </c>
+      <c r="S8" t="n">
+        <v>0.445943770310959</v>
+      </c>
+      <c r="T8" t="n">
+        <v>0.633076763588844</v>
+      </c>
+      <c r="U8" t="n">
+        <v>0.366396011516635</v>
+      </c>
+      <c r="V8" t="n">
+        <v>0.223571888867378</v>
+      </c>
+      <c r="W8" t="n">
+        <v>0.484556113960742</v>
+      </c>
+      <c r="X8" t="n">
+        <v>0.624276673154581</v>
+      </c>
+      <c r="Y8" t="n">
+        <v>0.303739821935569</v>
+      </c>
+      <c r="Z8" t="n">
+        <v>0.2316264693977</v>
+      </c>
+      <c r="AA8" t="n">
+        <v>0.42968802908603</v>
+      </c>
+      <c r="AB8" t="n">
+        <v>0.62359959476019</v>
+      </c>
+      <c r="AC8" t="n">
+        <v>0.332056255170512</v>
+      </c>
+      <c r="AD8" t="n">
+        <v>0.28310138799522</v>
+      </c>
+      <c r="AE8" t="n">
+        <v>0.250274841437632</v>
+      </c>
+      <c r="AF8" t="n">
+        <v>0.134567515396636</v>
+      </c>
+      <c r="AG8" t="s">
         <v>76</v>
       </c>
-      <c r="C8" t="s">
+      <c r="AH8" t="s">
         <v>77</v>
       </c>
-      <c r="D8" t="s">
+      <c r="AI8" t="s">
         <v>78</v>
       </c>
-      <c r="E8" t="n">
-        <v>40.364166</v>
-      </c>
-      <c r="F8" t="n">
-        <v>-74.783442</v>
-      </c>
-      <c r="G8" t="n">
-        <v>40.373815</v>
-      </c>
-      <c r="H8" t="n">
-        <v>-74.804523</v>
-      </c>
-      <c r="I8" t="n">
-        <v>40.354771</v>
-      </c>
-      <c r="J8" t="n">
-        <v>-74.762368</v>
-      </c>
-      <c r="K8" t="n">
-        <v>0.235294117647059</v>
-      </c>
-      <c r="L8" t="n">
-        <v>0.158270027965434</v>
-      </c>
-      <c r="M8" t="n">
-        <v>0.345098039215686</v>
-      </c>
-      <c r="N8" t="n">
-        <v>0.1328024853835</v>
-      </c>
-      <c r="O8" t="n">
-        <v>0.227450980392157</v>
-      </c>
-      <c r="P8" t="n">
-        <v>0.114245163447954</v>
-      </c>
-      <c r="Q8" t="n">
-        <v>0.223813620423603</v>
-      </c>
-      <c r="R8" t="n">
-        <v>0.115189278635276</v>
-      </c>
-      <c r="S8" t="n">
-        <v>0.40345144898967</v>
-      </c>
-      <c r="T8" t="n">
-        <v>0.586733777868203</v>
-      </c>
-      <c r="U8" t="n">
-        <v>0.328427491171107</v>
-      </c>
-      <c r="V8" t="n">
-        <v>0.194392081942834</v>
-      </c>
-      <c r="W8" t="n">
-        <v>0.465319231375064</v>
-      </c>
-      <c r="X8" t="n">
-        <v>0.568000171052044</v>
-      </c>
-      <c r="Y8" t="n">
-        <v>0.218584157153304</v>
-      </c>
-      <c r="Z8" t="n">
-        <v>0.143660635614015</v>
-      </c>
-      <c r="AA8" t="n">
-        <v>0.320048403622281</v>
-      </c>
-      <c r="AB8" t="n">
-        <v>0.496879536261878</v>
-      </c>
-      <c r="AC8" t="n">
-        <v>0.361272175751448</v>
-      </c>
-      <c r="AD8" t="n">
-        <v>0.265590587370163</v>
-      </c>
-      <c r="AE8" t="n">
-        <v>0.265239452155529</v>
-      </c>
-      <c r="AF8" t="n">
-        <v>0.107897784722861</v>
-      </c>
-      <c r="AG8" t="s">
+      <c r="AJ8" t="s">
         <v>79</v>
-      </c>
-      <c r="AH8" t="s">
-        <v>80</v>
-      </c>
-      <c r="AI8" t="s">
-        <v>81</v>
-      </c>
-      <c r="AJ8" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B9" t="s">
+        <v>81</v>
+      </c>
+      <c r="C9" t="s">
         <v>82</v>
       </c>
-      <c r="B9" t="s">
+      <c r="D9" t="s">
         <v>83</v>
       </c>
-      <c r="C9" t="s">
+      <c r="E9" t="n">
+        <v>40.364166</v>
+      </c>
+      <c r="F9" t="n">
+        <v>-74.783442</v>
+      </c>
+      <c r="G9" t="n">
+        <v>40.373815</v>
+      </c>
+      <c r="H9" t="n">
+        <v>-74.804523</v>
+      </c>
+      <c r="I9" t="n">
+        <v>40.354771</v>
+      </c>
+      <c r="J9" t="n">
+        <v>-74.762368</v>
+      </c>
+      <c r="K9" t="n">
+        <v>0.235294117647059</v>
+      </c>
+      <c r="L9" t="n">
+        <v>0.158270027965434</v>
+      </c>
+      <c r="M9" t="n">
+        <v>0.345098039215686</v>
+      </c>
+      <c r="N9" t="n">
+        <v>0.1328024853835</v>
+      </c>
+      <c r="O9" t="n">
+        <v>0.227450980392157</v>
+      </c>
+      <c r="P9" t="n">
+        <v>0.114245163447954</v>
+      </c>
+      <c r="Q9" t="n">
+        <v>0.223765038729398</v>
+      </c>
+      <c r="R9" t="n">
+        <v>0.11516503720601</v>
+      </c>
+      <c r="S9" t="n">
+        <v>0.40339530139506</v>
+      </c>
+      <c r="T9" t="n">
+        <v>0.586697227640182</v>
+      </c>
+      <c r="U9" t="n">
+        <v>0.328381216013129</v>
+      </c>
+      <c r="V9" t="n">
+        <v>0.194359024496223</v>
+      </c>
+      <c r="W9" t="n">
+        <v>0.465286404079278</v>
+      </c>
+      <c r="X9" t="n">
+        <v>0.567972954607</v>
+      </c>
+      <c r="Y9" t="n">
+        <v>0.218559554575643</v>
+      </c>
+      <c r="Z9" t="n">
+        <v>0.143643990005996</v>
+      </c>
+      <c r="AA9" t="n">
+        <v>0.320005016468611</v>
+      </c>
+      <c r="AB9" t="n">
+        <v>0.496834675217876</v>
+      </c>
+      <c r="AC9" t="n">
+        <v>0.361286882985569</v>
+      </c>
+      <c r="AD9" t="n">
+        <v>0.265465575880136</v>
+      </c>
+      <c r="AE9" t="n">
+        <v>0.265298281092012</v>
+      </c>
+      <c r="AF9" t="n">
+        <v>0.107949260042283</v>
+      </c>
+      <c r="AG9" t="s">
         <v>84</v>
       </c>
-      <c r="D9" t="s">
-        <v>78</v>
-      </c>
-      <c r="E9" t="n">
-        <v>40.338103</v>
-      </c>
-      <c r="F9" t="n">
-        <v>-74.661537</v>
-      </c>
-      <c r="G9" t="n">
-        <v>40.347688</v>
-      </c>
-      <c r="H9" t="n">
-        <v>-74.682536</v>
-      </c>
-      <c r="I9" t="n">
-        <v>40.328815</v>
-      </c>
-      <c r="J9" t="n">
-        <v>-74.640488</v>
-      </c>
-      <c r="K9" t="n">
-        <v>0.286274509803922</v>
-      </c>
-      <c r="L9" t="n">
-        <v>0.167347606554874</v>
-      </c>
-      <c r="M9" t="n">
-        <v>0.372549019607843</v>
-      </c>
-      <c r="N9" t="n">
-        <v>0.145400748965754</v>
-      </c>
-      <c r="O9" t="n">
-        <v>0.298039215686275</v>
-      </c>
-      <c r="P9" t="n">
-        <v>0.133731787612798</v>
-      </c>
-      <c r="Q9" t="n">
-        <v>0.280134259431886</v>
-      </c>
-      <c r="R9" t="n">
-        <v>0.164663258344967</v>
-      </c>
-      <c r="S9" t="n">
-        <v>0.445650204074035</v>
-      </c>
-      <c r="T9" t="n">
-        <v>0.646187491104984</v>
-      </c>
-      <c r="U9" t="n">
-        <v>0.370825658218107</v>
-      </c>
-      <c r="V9" t="n">
-        <v>0.229376073380913</v>
-      </c>
-      <c r="W9" t="n">
-        <v>0.490966044660862</v>
-      </c>
-      <c r="X9" t="n">
-        <v>0.632471479383723</v>
-      </c>
-      <c r="Y9" t="n">
-        <v>0.297335579653409</v>
-      </c>
-      <c r="Z9" t="n">
-        <v>0.230448343574166</v>
-      </c>
-      <c r="AA9" t="n">
-        <v>0.417237044355621</v>
-      </c>
-      <c r="AB9" t="n">
-        <v>0.617424586705571</v>
-      </c>
-      <c r="AC9" t="n">
-        <v>0.319018292122438</v>
-      </c>
-      <c r="AD9" t="n">
-        <v>0.315615405827742</v>
-      </c>
-      <c r="AE9" t="n">
-        <v>0.239485246805773</v>
-      </c>
-      <c r="AF9" t="n">
-        <v>0.125881055244048</v>
-      </c>
-      <c r="AG9" t="s">
-        <v>71</v>
-      </c>
       <c r="AH9" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="AI9" t="s">
-        <v>73</v>
+        <v>86</v>
       </c>
       <c r="AJ9" t="s">
-        <v>74</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="C10" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="D10" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="E10" t="n">
-        <v>40.358217</v>
+        <v>40.338103</v>
       </c>
       <c r="F10" t="n">
-        <v>-74.669685</v>
+        <v>-74.661537</v>
       </c>
       <c r="G10" t="n">
-        <v>40.369027</v>
+        <v>40.347688</v>
       </c>
       <c r="H10" t="n">
-        <v>-74.690723</v>
+        <v>-74.682536</v>
       </c>
       <c r="I10" t="n">
-        <v>40.348952</v>
+        <v>40.328815</v>
       </c>
       <c r="J10" t="n">
-        <v>-74.648488</v>
+        <v>-74.640488</v>
       </c>
       <c r="K10" t="n">
-        <v>0.274509803921569</v>
+        <v>0.286274509803922</v>
       </c>
       <c r="L10" t="n">
-        <v>0.162573166713187</v>
+        <v>0.167347606554874</v>
       </c>
       <c r="M10" t="n">
-        <v>0.364705882352941</v>
+        <v>0.372549019607843</v>
       </c>
       <c r="N10" t="n">
-        <v>0.141980590942576</v>
+        <v>0.145400748965754</v>
       </c>
       <c r="O10" t="n">
-        <v>0.294117647058824</v>
+        <v>0.298039215686275</v>
       </c>
       <c r="P10" t="n">
-        <v>0.14210989979474</v>
+        <v>0.133731787612798</v>
       </c>
       <c r="Q10" t="n">
-        <v>0.267661562189387</v>
+        <v>0.280134259431886</v>
       </c>
       <c r="R10" t="n">
-        <v>0.150240993285796</v>
+        <v>0.164663258344967</v>
       </c>
       <c r="S10" t="n">
-        <v>0.437783344077499</v>
+        <v>0.445650204074035</v>
       </c>
       <c r="T10" t="n">
-        <v>0.632509539636201</v>
+        <v>0.646187491104984</v>
       </c>
       <c r="U10" t="n">
-        <v>0.356086932939028</v>
+        <v>0.370825658218107</v>
       </c>
       <c r="V10" t="n">
-        <v>0.21820985583095</v>
+        <v>0.229376073380913</v>
       </c>
       <c r="W10" t="n">
-        <v>0.481264137518036</v>
+        <v>0.490966044660862</v>
       </c>
       <c r="X10" t="n">
-        <v>0.627157761440502</v>
+        <v>0.632471479383723</v>
       </c>
       <c r="Y10" t="n">
-        <v>0.289000651275803</v>
+        <v>0.297335579653409</v>
       </c>
       <c r="Z10" t="n">
-        <v>0.208345511780479</v>
+        <v>0.230448343574166</v>
       </c>
       <c r="AA10" t="n">
-        <v>0.416060480132297</v>
+        <v>0.417237044355621</v>
       </c>
       <c r="AB10" t="n">
-        <v>0.635005783590392</v>
+        <v>0.617424586705571</v>
       </c>
       <c r="AC10" t="n">
-        <v>0.366849894291755</v>
+        <v>0.319018292122438</v>
       </c>
       <c r="AD10" t="n">
-        <v>0.282005699053222</v>
+        <v>0.315615405827742</v>
       </c>
       <c r="AE10" t="n">
-        <v>0.236027208383123</v>
+        <v>0.239485246805773</v>
       </c>
       <c r="AF10" t="n">
-        <v>0.1151171982719</v>
+        <v>0.125881055244048</v>
       </c>
       <c r="AG10" t="s">
-        <v>89</v>
+        <v>76</v>
       </c>
       <c r="AH10" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="AI10" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="AJ10" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B11" t="s">
         <v>91</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>92</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>93</v>
       </c>
-      <c r="D11" t="s">
-        <v>88</v>
-      </c>
       <c r="E11" t="n">
-        <v>40.361706</v>
+        <v>40.358217</v>
       </c>
       <c r="F11" t="n">
-        <v>-74.737647</v>
+        <v>-74.669685</v>
       </c>
       <c r="G11" t="n">
-        <v>40.372664</v>
+        <v>40.369027</v>
       </c>
       <c r="H11" t="n">
-        <v>-74.758727</v>
+        <v>-74.690723</v>
       </c>
       <c r="I11" t="n">
-        <v>40.352399</v>
+        <v>40.348952</v>
       </c>
       <c r="J11" t="n">
-        <v>-74.716469</v>
+        <v>-74.648488</v>
       </c>
       <c r="K11" t="n">
-        <v>0.188235294117647</v>
+        <v>0.274509803921569</v>
       </c>
       <c r="L11" t="n">
-        <v>0.132743122622197</v>
+        <v>0.162573166713187</v>
       </c>
       <c r="M11" t="n">
-        <v>0.286274509803922</v>
+        <v>0.364705882352941</v>
       </c>
       <c r="N11" t="n">
-        <v>0.132355216070425</v>
+        <v>0.141980590942576</v>
       </c>
       <c r="O11" t="n">
-        <v>0.168627450980392</v>
+        <v>0.294117647058824</v>
       </c>
       <c r="P11" t="n">
-        <v>0.105567815528838</v>
+        <v>0.14210989979474</v>
       </c>
       <c r="Q11" t="n">
-        <v>0.1940861429368</v>
+        <v>0.267661562189387</v>
       </c>
       <c r="R11" t="n">
-        <v>0.0941360439372104</v>
+        <v>0.150240993285796</v>
       </c>
       <c r="S11" t="n">
-        <v>0.35784947516238</v>
+        <v>0.437783344077499</v>
       </c>
       <c r="T11" t="n">
-        <v>0.561962024880248</v>
+        <v>0.632509539636201</v>
       </c>
       <c r="U11" t="n">
-        <v>0.292419391378777</v>
+        <v>0.356086932939028</v>
       </c>
       <c r="V11" t="n">
-        <v>0.145948258779503</v>
+        <v>0.21820985583095</v>
       </c>
       <c r="W11" t="n">
-        <v>0.440513299223312</v>
+        <v>0.481264137518036</v>
       </c>
       <c r="X11" t="n">
-        <v>0.540075123195144</v>
+        <v>0.627157761440502</v>
       </c>
       <c r="Y11" t="n">
-        <v>0.17056172175429</v>
+        <v>0.289000651275803</v>
       </c>
       <c r="Z11" t="n">
-        <v>0.088518439690266</v>
+        <v>0.208345511780479</v>
       </c>
       <c r="AA11" t="n">
-        <v>0.27057007385756</v>
+        <v>0.416060480132297</v>
       </c>
       <c r="AB11" t="n">
-        <v>0.483013749612333</v>
+        <v>0.635005783590392</v>
       </c>
       <c r="AC11" t="n">
-        <v>0.420380549682875</v>
+        <v>0.366849894291755</v>
       </c>
       <c r="AD11" t="n">
-        <v>0.294696203695193</v>
+        <v>0.282005699053222</v>
       </c>
       <c r="AE11" t="n">
-        <v>0.232620645279897</v>
+        <v>0.236027208383123</v>
       </c>
       <c r="AF11" t="n">
-        <v>0.0523026013420351</v>
+        <v>0.1151171982719</v>
       </c>
       <c r="AG11" t="s">
-        <v>58</v>
+        <v>94</v>
       </c>
       <c r="AH11" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="AI11" t="s">
-        <v>41</v>
+        <v>78</v>
       </c>
       <c r="AJ11" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B12" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="D12" t="s">
-        <v>88</v>
+        <v>93</v>
       </c>
       <c r="E12" t="n">
-        <v>40.353131</v>
+        <v>40.361706</v>
       </c>
       <c r="F12" t="n">
-        <v>-74.719621</v>
+        <v>-74.737647</v>
       </c>
       <c r="G12" t="n">
-        <v>40.364018</v>
+        <v>40.372664</v>
       </c>
       <c r="H12" t="n">
-        <v>-74.740553</v>
+        <v>-74.758727</v>
       </c>
       <c r="I12" t="n">
-        <v>40.343789</v>
+        <v>40.352399</v>
       </c>
       <c r="J12" t="n">
-        <v>-74.698588</v>
+        <v>-74.716469</v>
       </c>
       <c r="K12" t="n">
         <v>0.188235294117647</v>
       </c>
       <c r="L12" t="n">
-        <v>0.138169660350124</v>
+        <v>0.132743122622197</v>
       </c>
       <c r="M12" t="n">
-        <v>0.282352941176471</v>
+        <v>0.286274509803922</v>
       </c>
       <c r="N12" t="n">
-        <v>0.133845667134806</v>
+        <v>0.132355216070425</v>
       </c>
       <c r="O12" t="n">
-        <v>0.172549019607843</v>
+        <v>0.168627450980392</v>
       </c>
       <c r="P12" t="n">
-        <v>0.108688456813032</v>
+        <v>0.105567815528838</v>
       </c>
       <c r="Q12" t="n">
-        <v>0.199002504762266</v>
+        <v>0.194175229085756</v>
       </c>
       <c r="R12" t="n">
-        <v>0.0986758383031911</v>
+        <v>0.094217821264732</v>
       </c>
       <c r="S12" t="n">
-        <v>0.370979619804829</v>
+        <v>0.357912616550107</v>
       </c>
       <c r="T12" t="n">
-        <v>0.590248151269788</v>
+        <v>0.561991989735164</v>
       </c>
       <c r="U12" t="n">
-        <v>0.293848871607279</v>
+        <v>0.29253305559382</v>
       </c>
       <c r="V12" t="n">
-        <v>0.154165729639159</v>
+        <v>0.14608090398064</v>
       </c>
       <c r="W12" t="n">
-        <v>0.443878615471349</v>
+        <v>0.440556063814605</v>
       </c>
       <c r="X12" t="n">
-        <v>0.565234844167891</v>
+        <v>0.540093864473596</v>
       </c>
       <c r="Y12" t="n">
-        <v>0.180590056290203</v>
+        <v>0.170628754708203</v>
       </c>
       <c r="Z12" t="n">
-        <v>0.108273825134283</v>
+        <v>0.0885917770457022</v>
       </c>
       <c r="AA12" t="n">
-        <v>0.279469764122718</v>
+        <v>0.270604297003346</v>
       </c>
       <c r="AB12" t="n">
-        <v>0.529532955028855</v>
+        <v>0.483060751288113</v>
       </c>
       <c r="AC12" t="n">
-        <v>0.403823880871404</v>
+        <v>0.41999264638294</v>
       </c>
       <c r="AD12" t="n">
-        <v>0.324106995128229</v>
+        <v>0.295216472102215</v>
       </c>
       <c r="AE12" t="n">
-        <v>0.222158286607225</v>
+        <v>0.232508502619726</v>
       </c>
       <c r="AF12" t="n">
-        <v>0.0499108373931428</v>
+        <v>0.052282378895119</v>
       </c>
       <c r="AG12" t="s">
-        <v>58</v>
+        <v>63</v>
       </c>
       <c r="AH12" t="s">
-        <v>48</v>
+        <v>99</v>
       </c>
       <c r="AI12" t="s">
         <v>41</v>
@@ -2134,332 +2146,332 @@
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C13" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="D13" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="E13" t="n">
-        <v>40.38491</v>
+        <v>40.353131</v>
       </c>
       <c r="F13" t="n">
-        <v>-74.75798</v>
+        <v>-74.719621</v>
       </c>
       <c r="G13" t="n">
-        <v>40.394606</v>
+        <v>40.364018</v>
       </c>
       <c r="H13" t="n">
-        <v>-74.779177</v>
+        <v>-74.740553</v>
       </c>
       <c r="I13" t="n">
-        <v>40.375683</v>
+        <v>40.343789</v>
       </c>
       <c r="J13" t="n">
-        <v>-74.736848</v>
+        <v>-74.698588</v>
       </c>
       <c r="K13" t="n">
-        <v>0.274509803921569</v>
+        <v>0.188235294117647</v>
       </c>
       <c r="L13" t="n">
-        <v>0.187551213212678</v>
+        <v>0.138169660350124</v>
       </c>
       <c r="M13" t="n">
-        <v>0.380392156862745</v>
+        <v>0.282352941176471</v>
       </c>
       <c r="N13" t="n">
-        <v>0.170926902286799</v>
+        <v>0.133845667134806</v>
       </c>
       <c r="O13" t="n">
-        <v>0.247058823529412</v>
+        <v>0.172549019607843</v>
       </c>
       <c r="P13" t="n">
-        <v>0.148443915207526</v>
+        <v>0.108688456813032</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.228363859815439</v>
+        <v>0.199002504762266</v>
       </c>
       <c r="R13" t="n">
-        <v>0.43157600065856</v>
+        <v>0.0986758383031911</v>
       </c>
       <c r="S13" t="n">
-        <v>0.102808511777867</v>
+        <v>0.370979619804829</v>
       </c>
       <c r="T13" t="n">
-        <v>0.603321216074059</v>
+        <v>0.590248151269788</v>
       </c>
       <c r="U13" t="n">
-        <v>0.329214996870535</v>
+        <v>0.293848871607279</v>
       </c>
       <c r="V13" t="n">
-        <v>0.496706030199968</v>
+        <v>0.154165729639159</v>
       </c>
       <c r="W13" t="n">
-        <v>0.156642335334534</v>
+        <v>0.443878615471349</v>
       </c>
       <c r="X13" t="n">
-        <v>0.611099243983062</v>
+        <v>0.565234844167891</v>
       </c>
       <c r="Y13" t="n">
-        <v>0.216509368565664</v>
+        <v>0.180590056290203</v>
       </c>
       <c r="Z13" t="n">
-        <v>0.351639680903773</v>
+        <v>0.108273825134283</v>
       </c>
       <c r="AA13" t="n">
-        <v>0.129206489040226</v>
+        <v>0.279469764122718</v>
       </c>
       <c r="AB13" t="n">
-        <v>0.524743338093403</v>
+        <v>0.529532955028855</v>
       </c>
       <c r="AC13" t="n">
-        <v>0.332025002298005</v>
+        <v>0.403823880871404</v>
       </c>
       <c r="AD13" t="n">
-        <v>0.24478904311058</v>
+        <v>0.324106995128229</v>
       </c>
       <c r="AE13" t="n">
-        <v>0.231515764316573</v>
+        <v>0.222158286607225</v>
       </c>
       <c r="AF13" t="n">
-        <v>0.191670190274841</v>
+        <v>0.0499108373931428</v>
       </c>
       <c r="AG13" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="AH13" t="s">
-        <v>102</v>
+        <v>54</v>
       </c>
       <c r="AI13" t="s">
-        <v>53</v>
+        <v>41</v>
       </c>
       <c r="AJ13" t="s">
-        <v>103</v>
+        <v>64</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
+        <v>103</v>
+      </c>
+      <c r="B14" t="s">
         <v>104</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
         <v>105</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>106</v>
       </c>
-      <c r="D14" t="s">
-        <v>101</v>
-      </c>
       <c r="E14" t="n">
-        <v>40.328281</v>
+        <v>40.38491</v>
       </c>
       <c r="F14" t="n">
-        <v>-74.804559</v>
+        <v>-74.75798</v>
       </c>
       <c r="G14" t="n">
-        <v>40.33784</v>
+        <v>40.394606</v>
       </c>
       <c r="H14" t="n">
-        <v>-74.825575</v>
+        <v>-74.779177</v>
       </c>
       <c r="I14" t="n">
-        <v>40.319148</v>
+        <v>40.375683</v>
       </c>
       <c r="J14" t="n">
-        <v>-74.783438</v>
+        <v>-74.736848</v>
       </c>
       <c r="K14" t="n">
-        <v>0.282352941176471</v>
+        <v>0.274509803921569</v>
       </c>
       <c r="L14" t="n">
-        <v>0.16522897235173</v>
+        <v>0.187551213212678</v>
       </c>
       <c r="M14" t="n">
-        <v>0.36078431372549</v>
+        <v>0.380392156862745</v>
       </c>
       <c r="N14" t="n">
-        <v>0.132527115261705</v>
+        <v>0.170926902286799</v>
       </c>
       <c r="O14" t="n">
         <v>0.247058823529412</v>
       </c>
       <c r="P14" t="n">
-        <v>0.125946290492155</v>
+        <v>0.148443915207526</v>
       </c>
       <c r="Q14" t="n">
-        <v>0.415040407962094</v>
+        <v>0.228363859815439</v>
       </c>
       <c r="R14" t="n">
-        <v>0.233873944664757</v>
+        <v>0.43157600065856</v>
       </c>
       <c r="S14" t="n">
-        <v>0.108223305346893</v>
+        <v>0.102808511777867</v>
       </c>
       <c r="T14" t="n">
-        <v>0.579102404647386</v>
+        <v>0.603321216074059</v>
       </c>
       <c r="U14" t="n">
-        <v>0.441550101742689</v>
+        <v>0.329214996870535</v>
       </c>
       <c r="V14" t="n">
-        <v>0.323920710338058</v>
+        <v>0.496706030199968</v>
       </c>
       <c r="W14" t="n">
-        <v>0.187500121892146</v>
+        <v>0.156642335334534</v>
       </c>
       <c r="X14" t="n">
-        <v>0.561522360690173</v>
+        <v>0.611099243983062</v>
       </c>
       <c r="Y14" t="n">
-        <v>0.329398239396863</v>
+        <v>0.216509368565664</v>
       </c>
       <c r="Z14" t="n">
-        <v>0.218969231435148</v>
+        <v>0.351639680903773</v>
       </c>
       <c r="AA14" t="n">
-        <v>0.144009569346886</v>
+        <v>0.129206489040226</v>
       </c>
       <c r="AB14" t="n">
-        <v>0.524350564735912</v>
+        <v>0.524743338093403</v>
       </c>
       <c r="AC14" t="n">
-        <v>0.327281919294053</v>
+        <v>0.332025002298005</v>
       </c>
       <c r="AD14" t="n">
-        <v>0.292311793363361</v>
+        <v>0.24478904311058</v>
       </c>
       <c r="AE14" t="n">
-        <v>0.266156815883813</v>
+        <v>0.231515764316573</v>
       </c>
       <c r="AF14" t="n">
-        <v>0.114249471458774</v>
+        <v>0.191670190274841</v>
       </c>
       <c r="AG14" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="AH14" t="s">
-        <v>79</v>
+        <v>107</v>
       </c>
       <c r="AI14" t="s">
-        <v>80</v>
+        <v>58</v>
       </c>
       <c r="AJ14" t="s">
-        <v>59</v>
+        <v>108</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D15" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="E15" t="n">
-        <v>40.321026</v>
+        <v>40.328281</v>
       </c>
       <c r="F15" t="n">
-        <v>-74.78868</v>
+        <v>-74.804559</v>
       </c>
       <c r="G15" t="n">
-        <v>40.330632</v>
+        <v>40.33784</v>
       </c>
       <c r="H15" t="n">
-        <v>-74.809579</v>
+        <v>-74.825575</v>
       </c>
       <c r="I15" t="n">
-        <v>40.311546</v>
+        <v>40.319148</v>
       </c>
       <c r="J15" t="n">
-        <v>-74.767619</v>
+        <v>-74.783438</v>
       </c>
       <c r="K15" t="n">
-        <v>0.254901960784314</v>
+        <v>0.282352941176471</v>
       </c>
       <c r="L15" t="n">
-        <v>0.158383812480717</v>
+        <v>0.16522897235173</v>
       </c>
       <c r="M15" t="n">
-        <v>0.345098039215686</v>
+        <v>0.36078431372549</v>
       </c>
       <c r="N15" t="n">
-        <v>0.13176240944685</v>
+        <v>0.132527115261705</v>
       </c>
       <c r="O15" t="n">
-        <v>0.231372549019608</v>
+        <v>0.247058823529412</v>
       </c>
       <c r="P15" t="n">
-        <v>0.1205155271785</v>
+        <v>0.125946290492155</v>
       </c>
       <c r="Q15" t="n">
-        <v>0.381367021957964</v>
+        <v>0.414175494233639</v>
       </c>
       <c r="R15" t="n">
-        <v>0.215405547415513</v>
+        <v>0.232701159939183</v>
       </c>
       <c r="S15" t="n">
-        <v>0.104149783428828</v>
+        <v>0.107783493729375</v>
       </c>
       <c r="T15" t="n">
-        <v>0.568970144359676</v>
+        <v>0.578749713273707</v>
       </c>
       <c r="U15" t="n">
-        <v>0.436413829874851</v>
+        <v>0.441110565830947</v>
       </c>
       <c r="V15" t="n">
-        <v>0.312425183035085</v>
+        <v>0.32290874320542</v>
       </c>
       <c r="W15" t="n">
-        <v>0.182392710736149</v>
+        <v>0.186939896796217</v>
       </c>
       <c r="X15" t="n">
-        <v>0.552816371783496</v>
+        <v>0.561162808138611</v>
       </c>
       <c r="Y15" t="n">
-        <v>0.310592356622423</v>
+        <v>0.32877186950485</v>
       </c>
       <c r="Z15" t="n">
-        <v>0.213408306540654</v>
+        <v>0.21831404298414</v>
       </c>
       <c r="AA15" t="n">
-        <v>0.146799317391483</v>
+        <v>0.143738057646491</v>
       </c>
       <c r="AB15" t="n">
-        <v>0.511936358166229</v>
+        <v>0.523786626049584</v>
       </c>
       <c r="AC15" t="n">
-        <v>0.312074639213163</v>
+        <v>0.328995312069124</v>
       </c>
       <c r="AD15" t="n">
-        <v>0.311462450592885</v>
+        <v>0.29201581027668</v>
       </c>
       <c r="AE15" t="n">
-        <v>0.258505377332475</v>
+        <v>0.264112510341024</v>
       </c>
       <c r="AF15" t="n">
-        <v>0.117957532861476</v>
+        <v>0.114876367313172</v>
       </c>
       <c r="AG15" t="s">
-        <v>110</v>
+        <v>86</v>
       </c>
       <c r="AH15" t="s">
-        <v>111</v>
+        <v>84</v>
       </c>
       <c r="AI15" t="s">
-        <v>42</v>
+        <v>85</v>
       </c>
       <c r="AJ15" t="s">
-        <v>49</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16">
@@ -2473,213 +2485,213 @@
         <v>114</v>
       </c>
       <c r="D16" t="s">
+        <v>106</v>
+      </c>
+      <c r="E16" t="n">
+        <v>40.321026</v>
+      </c>
+      <c r="F16" t="n">
+        <v>-74.78868</v>
+      </c>
+      <c r="G16" t="n">
+        <v>40.330632</v>
+      </c>
+      <c r="H16" t="n">
+        <v>-74.809579</v>
+      </c>
+      <c r="I16" t="n">
+        <v>40.311546</v>
+      </c>
+      <c r="J16" t="n">
+        <v>-74.767619</v>
+      </c>
+      <c r="K16" t="n">
+        <v>0.254901960784314</v>
+      </c>
+      <c r="L16" t="n">
+        <v>0.158383812480717</v>
+      </c>
+      <c r="M16" t="n">
+        <v>0.345098039215686</v>
+      </c>
+      <c r="N16" t="n">
+        <v>0.13176240944685</v>
+      </c>
+      <c r="O16" t="n">
+        <v>0.231372549019608</v>
+      </c>
+      <c r="P16" t="n">
+        <v>0.1205155271785</v>
+      </c>
+      <c r="Q16" t="n">
+        <v>0.381367021957964</v>
+      </c>
+      <c r="R16" t="n">
+        <v>0.215405547415513</v>
+      </c>
+      <c r="S16" t="n">
+        <v>0.104149783428828</v>
+      </c>
+      <c r="T16" t="n">
+        <v>0.568970144359676</v>
+      </c>
+      <c r="U16" t="n">
+        <v>0.436413829874851</v>
+      </c>
+      <c r="V16" t="n">
+        <v>0.312425183035085</v>
+      </c>
+      <c r="W16" t="n">
+        <v>0.182392710736149</v>
+      </c>
+      <c r="X16" t="n">
+        <v>0.552816371783496</v>
+      </c>
+      <c r="Y16" t="n">
+        <v>0.310592356622423</v>
+      </c>
+      <c r="Z16" t="n">
+        <v>0.213408306540654</v>
+      </c>
+      <c r="AA16" t="n">
+        <v>0.146799317391483</v>
+      </c>
+      <c r="AB16" t="n">
+        <v>0.511936358166229</v>
+      </c>
+      <c r="AC16" t="n">
+        <v>0.312074639213163</v>
+      </c>
+      <c r="AD16" t="n">
+        <v>0.311462450592885</v>
+      </c>
+      <c r="AE16" t="n">
+        <v>0.258505377332475</v>
+      </c>
+      <c r="AF16" t="n">
+        <v>0.117957532861476</v>
+      </c>
+      <c r="AG16" t="s">
         <v>115</v>
       </c>
-      <c r="E16" t="n">
-        <v>40.343974</v>
-      </c>
-      <c r="F16" t="n">
-        <v>-74.656639</v>
-      </c>
-      <c r="G16" t="n">
-        <v>40.354959</v>
-      </c>
-      <c r="H16" t="n">
-        <v>-74.677713</v>
-      </c>
-      <c r="I16" t="n">
-        <v>40.334793</v>
-      </c>
-      <c r="J16" t="n">
-        <v>-74.635716</v>
-      </c>
-      <c r="K16" t="n">
-        <v>0.305882352941176</v>
-      </c>
-      <c r="L16" t="n">
-        <v>0.167543143460215</v>
-      </c>
-      <c r="M16" t="n">
-        <v>0.384313725490196</v>
-      </c>
-      <c r="N16" t="n">
-        <v>0.145906563716664</v>
-      </c>
-      <c r="O16" t="n">
-        <v>0.313725490196078</v>
-      </c>
-      <c r="P16" t="n">
-        <v>0.1384357166309</v>
-      </c>
-      <c r="Q16" t="n">
-        <v>0.288346720349506</v>
-      </c>
-      <c r="R16" t="n">
-        <v>0.168390126059778</v>
-      </c>
-      <c r="S16" t="n">
-        <v>0.454040793920364</v>
-      </c>
-      <c r="T16" t="n">
-        <v>0.649498305401255</v>
-      </c>
-      <c r="U16" t="n">
-        <v>0.374038405313683</v>
-      </c>
-      <c r="V16" t="n">
-        <v>0.227670648318794</v>
-      </c>
-      <c r="W16" t="n">
-        <v>0.490080066013682</v>
-      </c>
-      <c r="X16" t="n">
-        <v>0.637245095414923</v>
-      </c>
-      <c r="Y16" t="n">
-        <v>0.305989040406259</v>
-      </c>
-      <c r="Z16" t="n">
-        <v>0.233742913421416</v>
-      </c>
-      <c r="AA16" t="n">
-        <v>0.435221311859108</v>
-      </c>
-      <c r="AB16" t="n">
-        <v>0.629861898972686</v>
-      </c>
-      <c r="AC16" t="n">
-        <v>0.331659159849251</v>
-      </c>
-      <c r="AD16" t="n">
-        <v>0.289896130159022</v>
-      </c>
-      <c r="AE16" t="n">
-        <v>0.247952936850813</v>
-      </c>
-      <c r="AF16" t="n">
-        <v>0.130491773140914</v>
-      </c>
-      <c r="AG16" t="s">
-        <v>71</v>
-      </c>
       <c r="AH16" t="s">
-        <v>72</v>
+        <v>47</v>
       </c>
       <c r="AI16" t="s">
-        <v>116</v>
+        <v>42</v>
       </c>
       <c r="AJ16" t="s">
-        <v>117</v>
+        <v>49</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
+        <v>116</v>
+      </c>
+      <c r="B17" t="s">
+        <v>117</v>
+      </c>
+      <c r="C17" t="s">
         <v>118</v>
       </c>
-      <c r="B17" t="s">
+      <c r="D17" t="s">
         <v>119</v>
       </c>
-      <c r="C17" t="s">
+      <c r="E17" t="n">
+        <v>40.343974</v>
+      </c>
+      <c r="F17" t="n">
+        <v>-74.656639</v>
+      </c>
+      <c r="G17" t="n">
+        <v>40.354959</v>
+      </c>
+      <c r="H17" t="n">
+        <v>-74.677713</v>
+      </c>
+      <c r="I17" t="n">
+        <v>40.334793</v>
+      </c>
+      <c r="J17" t="n">
+        <v>-74.635716</v>
+      </c>
+      <c r="K17" t="n">
+        <v>0.305882352941176</v>
+      </c>
+      <c r="L17" t="n">
+        <v>0.167543143460215</v>
+      </c>
+      <c r="M17" t="n">
+        <v>0.384313725490196</v>
+      </c>
+      <c r="N17" t="n">
+        <v>0.145906563716664</v>
+      </c>
+      <c r="O17" t="n">
+        <v>0.313725490196078</v>
+      </c>
+      <c r="P17" t="n">
+        <v>0.1384357166309</v>
+      </c>
+      <c r="Q17" t="n">
+        <v>0.2882036988913</v>
+      </c>
+      <c r="R17" t="n">
+        <v>0.168325602256577</v>
+      </c>
+      <c r="S17" t="n">
+        <v>0.453827762669032</v>
+      </c>
+      <c r="T17" t="n">
+        <v>0.649365524787776</v>
+      </c>
+      <c r="U17" t="n">
+        <v>0.373905081940544</v>
+      </c>
+      <c r="V17" t="n">
+        <v>0.227583929269188</v>
+      </c>
+      <c r="W17" t="n">
+        <v>0.489954842349313</v>
+      </c>
+      <c r="X17" t="n">
+        <v>0.637110622826983</v>
+      </c>
+      <c r="Y17" t="n">
+        <v>0.305895482295654</v>
+      </c>
+      <c r="Z17" t="n">
+        <v>0.233708963704582</v>
+      </c>
+      <c r="AA17" t="n">
+        <v>0.435046167645118</v>
+      </c>
+      <c r="AB17" t="n">
+        <v>0.629673243059598</v>
+      </c>
+      <c r="AC17" t="n">
+        <v>0.331660998253516</v>
+      </c>
+      <c r="AD17" t="n">
+        <v>0.289572571008365</v>
+      </c>
+      <c r="AE17" t="n">
+        <v>0.248048533872599</v>
+      </c>
+      <c r="AF17" t="n">
+        <v>0.130717896865521</v>
+      </c>
+      <c r="AG17" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH17" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI17" t="s">
         <v>120</v>
       </c>
-      <c r="D17" t="s">
-        <v>115</v>
-      </c>
-      <c r="E17" t="n">
-        <v>40.342717</v>
-      </c>
-      <c r="F17" t="n">
-        <v>-74.650305</v>
-      </c>
-      <c r="G17" t="n">
-        <v>40.353617</v>
-      </c>
-      <c r="H17" t="n">
-        <v>-74.671335</v>
-      </c>
-      <c r="I17" t="n">
-        <v>40.333492</v>
-      </c>
-      <c r="J17" t="n">
-        <v>-74.629285</v>
-      </c>
-      <c r="K17" t="n">
-        <v>0.317647058823529</v>
-      </c>
-      <c r="L17" t="n">
-        <v>0.169709864689101</v>
-      </c>
-      <c r="M17" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="N17" t="n">
-        <v>0.148531536935067</v>
-      </c>
-      <c r="O17" t="n">
-        <v>0.32156862745098</v>
-      </c>
-      <c r="P17" t="n">
-        <v>0.138730638706018</v>
-      </c>
-      <c r="Q17" t="n">
-        <v>0.292485254009982</v>
-      </c>
-      <c r="R17" t="n">
-        <v>0.170953388221756</v>
-      </c>
-      <c r="S17" t="n">
-        <v>0.45861257162221</v>
-      </c>
-      <c r="T17" t="n">
-        <v>0.653141707058603</v>
-      </c>
-      <c r="U17" t="n">
-        <v>0.381564529542702</v>
-      </c>
-      <c r="V17" t="n">
-        <v>0.227219813435469</v>
-      </c>
-      <c r="W17" t="n">
-        <v>0.494421844158163</v>
-      </c>
-      <c r="X17" t="n">
-        <v>0.640496481013311</v>
-      </c>
-      <c r="Y17" t="n">
-        <v>0.309013968191812</v>
-      </c>
-      <c r="Z17" t="n">
-        <v>0.237773962004343</v>
-      </c>
-      <c r="AA17" t="n">
-        <v>0.436045381692298</v>
-      </c>
-      <c r="AB17" t="n">
-        <v>0.630067369677396</v>
-      </c>
-      <c r="AC17" t="n">
-        <v>0.322654655758801</v>
-      </c>
-      <c r="AD17" t="n">
-        <v>0.282461623310966</v>
-      </c>
-      <c r="AE17" t="n">
-        <v>0.257404173177682</v>
-      </c>
-      <c r="AF17" t="n">
-        <v>0.137479547752551</v>
-      </c>
-      <c r="AG17" t="s">
+      <c r="AJ17" t="s">
         <v>121</v>
-      </c>
-      <c r="AH17" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI17" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ17" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="18">
@@ -2693,213 +2705,213 @@
         <v>124</v>
       </c>
       <c r="D18" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E18" t="n">
-        <v>40.345588</v>
+        <v>40.342717</v>
       </c>
       <c r="F18" t="n">
-        <v>-74.654241</v>
+        <v>-74.650305</v>
       </c>
       <c r="G18" t="n">
-        <v>40.356659</v>
+        <v>40.353617</v>
       </c>
       <c r="H18" t="n">
-        <v>-74.675203</v>
+        <v>-74.671335</v>
       </c>
       <c r="I18" t="n">
-        <v>40.336579</v>
+        <v>40.333492</v>
       </c>
       <c r="J18" t="n">
-        <v>-74.633262</v>
+        <v>-74.629285</v>
       </c>
       <c r="K18" t="n">
-        <v>0.305882352941176</v>
+        <v>0.317647058823529</v>
       </c>
       <c r="L18" t="n">
-        <v>0.165427329198988</v>
+        <v>0.169709864689101</v>
       </c>
       <c r="M18" t="n">
-        <v>0.384313725490196</v>
+        <v>0.4</v>
       </c>
       <c r="N18" t="n">
-        <v>0.145041657721354</v>
+        <v>0.148531536935067</v>
       </c>
       <c r="O18" t="n">
-        <v>0.317647058823529</v>
+        <v>0.32156862745098</v>
       </c>
       <c r="P18" t="n">
-        <v>0.138051140260026</v>
+        <v>0.138730638706018</v>
       </c>
       <c r="Q18" t="n">
-        <v>0.285956974504185</v>
+        <v>0.292485254009982</v>
       </c>
       <c r="R18" t="n">
-        <v>0.167256042265955</v>
+        <v>0.170953388221756</v>
       </c>
       <c r="S18" t="n">
-        <v>0.448686538735146</v>
+        <v>0.45861257162221</v>
       </c>
       <c r="T18" t="n">
-        <v>0.637845547458932</v>
+        <v>0.653141707058603</v>
       </c>
       <c r="U18" t="n">
-        <v>0.37105325487389</v>
+        <v>0.381564529542702</v>
       </c>
       <c r="V18" t="n">
-        <v>0.224744019086729</v>
+        <v>0.227219813435469</v>
       </c>
       <c r="W18" t="n">
-        <v>0.48581713864281</v>
+        <v>0.494421844158163</v>
       </c>
       <c r="X18" t="n">
-        <v>0.627750417155787</v>
+        <v>0.640496481013311</v>
       </c>
       <c r="Y18" t="n">
-        <v>0.306066571224039</v>
+        <v>0.309013968191812</v>
       </c>
       <c r="Z18" t="n">
-        <v>0.234403095494846</v>
+        <v>0.237773962004343</v>
       </c>
       <c r="AA18" t="n">
-        <v>0.433734433207618</v>
+        <v>0.436045381692298</v>
       </c>
       <c r="AB18" t="n">
-        <v>0.624350838928254</v>
+        <v>0.630067369677396</v>
       </c>
       <c r="AC18" t="n">
-        <v>0.328736097067745</v>
+        <v>0.322654655758801</v>
       </c>
       <c r="AD18" t="n">
-        <v>0.286719367588933</v>
+        <v>0.282461623310966</v>
       </c>
       <c r="AE18" t="n">
-        <v>0.248294880044122</v>
+        <v>0.257404173177682</v>
       </c>
       <c r="AF18" t="n">
-        <v>0.1362496552992</v>
+        <v>0.137479547752551</v>
       </c>
       <c r="AG18" t="s">
-        <v>71</v>
+        <v>125</v>
       </c>
       <c r="AH18" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="AI18" t="s">
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="AJ18" t="s">
-        <v>74</v>
+        <v>121</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="D19" t="s">
-        <v>115</v>
+        <v>119</v>
       </c>
       <c r="E19" t="n">
-        <v>40.334348</v>
+        <v>40.345588</v>
       </c>
       <c r="F19" t="n">
-        <v>-74.647146</v>
+        <v>-74.654241</v>
       </c>
       <c r="G19" t="n">
-        <v>40.345334</v>
+        <v>40.356659</v>
       </c>
       <c r="H19" t="n">
-        <v>-74.668232</v>
+        <v>-74.675203</v>
       </c>
       <c r="I19" t="n">
-        <v>40.325165</v>
+        <v>40.336579</v>
       </c>
       <c r="J19" t="n">
-        <v>-74.626075</v>
+        <v>-74.633262</v>
       </c>
       <c r="K19" t="n">
         <v>0.305882352941176</v>
       </c>
       <c r="L19" t="n">
-        <v>0.171906193075733</v>
+        <v>0.165427329198988</v>
       </c>
       <c r="M19" t="n">
-        <v>0.4</v>
+        <v>0.384313725490196</v>
       </c>
       <c r="N19" t="n">
-        <v>0.147968122912027</v>
+        <v>0.145041657721354</v>
       </c>
       <c r="O19" t="n">
-        <v>0.313725490196078</v>
+        <v>0.317647058823529</v>
       </c>
       <c r="P19" t="n">
-        <v>0.136295469367197</v>
+        <v>0.138051140260026</v>
       </c>
       <c r="Q19" t="n">
-        <v>0.17302914627532</v>
+        <v>0.286016592112501</v>
       </c>
       <c r="R19" t="n">
-        <v>0.291492232767294</v>
+        <v>0.167288473764473</v>
       </c>
       <c r="S19" t="n">
-        <v>0.462848116278828</v>
+        <v>0.44872680067695</v>
       </c>
       <c r="T19" t="n">
-        <v>0.655632176030561</v>
+        <v>0.63786851871112</v>
       </c>
       <c r="U19" t="n">
-        <v>0.238589797195482</v>
+        <v>0.371105803729398</v>
       </c>
       <c r="V19" t="n">
-        <v>0.389570586544744</v>
+        <v>0.224797174540718</v>
       </c>
       <c r="W19" t="n">
-        <v>0.500561271788249</v>
+        <v>0.485839531798945</v>
       </c>
       <c r="X19" t="n">
-        <v>0.642023248312885</v>
+        <v>0.62777436835477</v>
       </c>
       <c r="Y19" t="n">
-        <v>0.239815844608889</v>
+        <v>0.306103722969579</v>
       </c>
       <c r="Z19" t="n">
-        <v>0.307033922557406</v>
+        <v>0.234419441491841</v>
       </c>
       <c r="AA19" t="n">
-        <v>0.430912748478509</v>
+        <v>0.43377637025115</v>
       </c>
       <c r="AB19" t="n">
-        <v>0.6264441264314</v>
+        <v>0.624375089811605</v>
       </c>
       <c r="AC19" t="n">
-        <v>0.319413549039434</v>
+        <v>0.32863682323743</v>
       </c>
       <c r="AD19" t="n">
-        <v>0.296385697214818</v>
+        <v>0.286901369611178</v>
       </c>
       <c r="AE19" t="n">
-        <v>0.251655483040721</v>
+        <v>0.248248919937494</v>
       </c>
       <c r="AF19" t="n">
-        <v>0.132545270705028</v>
+        <v>0.136212887213898</v>
       </c>
       <c r="AG19" t="s">
-        <v>58</v>
+        <v>76</v>
       </c>
       <c r="AH19" t="s">
-        <v>121</v>
+        <v>77</v>
       </c>
       <c r="AI19" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="AJ19" t="s">
-        <v>117</v>
+        <v>79</v>
       </c>
     </row>
     <row r="20">
@@ -2913,103 +2925,213 @@
         <v>131</v>
       </c>
       <c r="D20" t="s">
-        <v>132</v>
+        <v>119</v>
       </c>
       <c r="E20" t="n">
-        <v>40.35151</v>
+        <v>40.334348</v>
       </c>
       <c r="F20" t="n">
-        <v>-74.660325</v>
+        <v>-74.647146</v>
       </c>
       <c r="G20" t="n">
-        <v>40.357259</v>
+        <v>40.345334</v>
       </c>
       <c r="H20" t="n">
-        <v>-74.671573</v>
+        <v>-74.668232</v>
       </c>
       <c r="I20" t="n">
-        <v>40.34662</v>
+        <v>40.325165</v>
       </c>
       <c r="J20" t="n">
-        <v>-74.648996</v>
+        <v>-74.626075</v>
       </c>
       <c r="K20" t="n">
-        <v>0.298039215686275</v>
+        <v>0.305882352941176</v>
       </c>
       <c r="L20" t="n">
-        <v>0.163940995974375</v>
+        <v>0.171906193075733</v>
       </c>
       <c r="M20" t="n">
-        <v>0.380392156862745</v>
+        <v>0.4</v>
       </c>
       <c r="N20" t="n">
-        <v>0.144352586153883</v>
+        <v>0.147968122912027</v>
       </c>
       <c r="O20" t="n">
         <v>0.313725490196078</v>
       </c>
       <c r="P20" t="n">
+        <v>0.136295469367197</v>
+      </c>
+      <c r="Q20" t="n">
+        <v>0.17302914627532</v>
+      </c>
+      <c r="R20" t="n">
+        <v>0.291492232767294</v>
+      </c>
+      <c r="S20" t="n">
+        <v>0.462848116278828</v>
+      </c>
+      <c r="T20" t="n">
+        <v>0.655632176030561</v>
+      </c>
+      <c r="U20" t="n">
+        <v>0.238589797195482</v>
+      </c>
+      <c r="V20" t="n">
+        <v>0.389570586544744</v>
+      </c>
+      <c r="W20" t="n">
+        <v>0.500561271788249</v>
+      </c>
+      <c r="X20" t="n">
+        <v>0.642023248312885</v>
+      </c>
+      <c r="Y20" t="n">
+        <v>0.239815844608889</v>
+      </c>
+      <c r="Z20" t="n">
+        <v>0.307033922557406</v>
+      </c>
+      <c r="AA20" t="n">
+        <v>0.430912748478509</v>
+      </c>
+      <c r="AB20" t="n">
+        <v>0.6264441264314</v>
+      </c>
+      <c r="AC20" t="n">
+        <v>0.319413549039434</v>
+      </c>
+      <c r="AD20" t="n">
+        <v>0.296385697214818</v>
+      </c>
+      <c r="AE20" t="n">
+        <v>0.251655483040721</v>
+      </c>
+      <c r="AF20" t="n">
+        <v>0.132545270705028</v>
+      </c>
+      <c r="AG20" t="s">
+        <v>63</v>
+      </c>
+      <c r="AH20" t="s">
+        <v>125</v>
+      </c>
+      <c r="AI20" t="s">
+        <v>132</v>
+      </c>
+      <c r="AJ20" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>133</v>
+      </c>
+      <c r="B21" t="s">
+        <v>134</v>
+      </c>
+      <c r="C21" t="s">
+        <v>135</v>
+      </c>
+      <c r="D21" t="s">
+        <v>136</v>
+      </c>
+      <c r="E21" t="n">
+        <v>40.35151</v>
+      </c>
+      <c r="F21" t="n">
+        <v>-74.660325</v>
+      </c>
+      <c r="G21" t="n">
+        <v>40.357259</v>
+      </c>
+      <c r="H21" t="n">
+        <v>-74.671573</v>
+      </c>
+      <c r="I21" t="n">
+        <v>40.34662</v>
+      </c>
+      <c r="J21" t="n">
+        <v>-74.648996</v>
+      </c>
+      <c r="K21" t="n">
+        <v>0.298039215686275</v>
+      </c>
+      <c r="L21" t="n">
+        <v>0.163940995974375</v>
+      </c>
+      <c r="M21" t="n">
+        <v>0.380392156862745</v>
+      </c>
+      <c r="N21" t="n">
+        <v>0.144352586153883</v>
+      </c>
+      <c r="O21" t="n">
+        <v>0.313725490196078</v>
+      </c>
+      <c r="P21" t="n">
         <v>0.141369147301135</v>
       </c>
-      <c r="Q20" t="n">
-        <v>0.290054309778663</v>
-      </c>
-      <c r="R20" t="n">
-        <v>0.167018335101561</v>
-      </c>
-      <c r="S20" t="n">
-        <v>0.458670411202548</v>
-      </c>
-      <c r="T20" t="n">
-        <v>0.643780422542729</v>
-      </c>
-      <c r="U20" t="n">
-        <v>0.373545394552962</v>
-      </c>
-      <c r="V20" t="n">
-        <v>0.229170677153524</v>
-      </c>
-      <c r="W20" t="n">
-        <v>0.493155287112214</v>
-      </c>
-      <c r="X20" t="n">
-        <v>0.63821369359121</v>
-      </c>
-      <c r="Y20" t="n">
-        <v>0.309083010639517</v>
-      </c>
-      <c r="Z20" t="n">
-        <v>0.230508165471853</v>
-      </c>
-      <c r="AA20" t="n">
-        <v>0.439155055375326</v>
-      </c>
-      <c r="AB20" t="n">
-        <v>0.648456573677854</v>
-      </c>
-      <c r="AC20" t="n">
-        <v>0.34112510341024</v>
-      </c>
-      <c r="AD20" t="n">
-        <v>0.298858350951374</v>
-      </c>
-      <c r="AE20" t="n">
-        <v>0.243283390017465</v>
-      </c>
-      <c r="AF20" t="n">
-        <v>0.116733155620921</v>
-      </c>
-      <c r="AG20" t="s">
-        <v>71</v>
-      </c>
-      <c r="AH20" t="s">
-        <v>72</v>
-      </c>
-      <c r="AI20" t="s">
-        <v>116</v>
-      </c>
-      <c r="AJ20" t="s">
-        <v>117</v>
+      <c r="Q21" t="n">
+        <v>0.290321210612135</v>
+      </c>
+      <c r="R21" t="n">
+        <v>0.16710471678844</v>
+      </c>
+      <c r="S21" t="n">
+        <v>0.459097965957467</v>
+      </c>
+      <c r="T21" t="n">
+        <v>0.644182291196637</v>
+      </c>
+      <c r="U21" t="n">
+        <v>0.373786888386109</v>
+      </c>
+      <c r="V21" t="n">
+        <v>0.229292852656006</v>
+      </c>
+      <c r="W21" t="n">
+        <v>0.493405262816828</v>
+      </c>
+      <c r="X21" t="n">
+        <v>0.638586518479793</v>
+      </c>
+      <c r="Y21" t="n">
+        <v>0.309250446621567</v>
+      </c>
+      <c r="Z21" t="n">
+        <v>0.23056136025559</v>
+      </c>
+      <c r="AA21" t="n">
+        <v>0.439617835320568</v>
+      </c>
+      <c r="AB21" t="n">
+        <v>0.648854966093214</v>
+      </c>
+      <c r="AC21" t="n">
+        <v>0.341365934368968</v>
+      </c>
+      <c r="AD21" t="n">
+        <v>0.299321628826179</v>
+      </c>
+      <c r="AE21" t="n">
+        <v>0.243075650335509</v>
+      </c>
+      <c r="AF21" t="n">
+        <v>0.116236786469345</v>
+      </c>
+      <c r="AG21" t="s">
+        <v>76</v>
+      </c>
+      <c r="AH21" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI21" t="s">
+        <v>120</v>
+      </c>
+      <c r="AJ21" t="s">
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -3028,10 +3150,10 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>133</v>
+        <v>137</v>
       </c>
       <c r="B1" t="s">
-        <v>134</v>
+        <v>138</v>
       </c>
     </row>
     <row r="2">
@@ -3039,7 +3161,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>135</v>
+        <v>139</v>
       </c>
     </row>
     <row r="3">
@@ -3047,7 +3169,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>136</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4">
@@ -3055,7 +3177,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>137</v>
+        <v>141</v>
       </c>
     </row>
     <row r="5">
@@ -3063,7 +3185,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6">
@@ -3071,7 +3193,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>139</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7">
@@ -3079,7 +3201,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>140</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8">
@@ -3087,7 +3209,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>141</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9">
@@ -3095,7 +3217,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10">
@@ -3103,7 +3225,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>143</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11">
@@ -3111,7 +3233,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>144</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12">
@@ -3119,7 +3241,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>145</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13">
@@ -3127,7 +3249,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14">
@@ -3135,7 +3257,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>147</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15">
@@ -3143,7 +3265,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
     </row>
     <row r="16">
@@ -3151,7 +3273,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>149</v>
+        <v>153</v>
       </c>
     </row>
     <row r="17">
@@ -3159,7 +3281,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>150</v>
+        <v>154</v>
       </c>
     </row>
     <row r="18">
@@ -3167,7 +3289,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="19">
@@ -3175,7 +3297,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="20">
@@ -3183,7 +3305,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="21">
@@ -3191,7 +3313,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>151</v>
+        <v>155</v>
       </c>
     </row>
     <row r="22">
@@ -3199,7 +3321,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="23">
@@ -3207,7 +3329,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="24">
@@ -3215,7 +3337,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="25">
@@ -3223,7 +3345,7 @@
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
     </row>
     <row r="26">
@@ -3231,7 +3353,7 @@
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="27">
@@ -3239,7 +3361,7 @@
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="28">
@@ -3247,7 +3369,7 @@
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="29">
@@ -3255,7 +3377,7 @@
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>153</v>
+        <v>157</v>
       </c>
     </row>
     <row r="30">
@@ -3263,7 +3385,7 @@
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="31">
@@ -3271,7 +3393,7 @@
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32">
@@ -3279,7 +3401,7 @@
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="33">
@@ -3287,7 +3409,7 @@
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>154</v>
+        <v>158</v>
       </c>
     </row>
     <row r="34">
@@ -3295,7 +3417,7 @@
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="35">
@@ -3303,7 +3425,7 @@
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="36">
@@ -3311,7 +3433,7 @@
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
     <row r="37">
@@ -3319,7 +3441,7 @@
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>